<commit_message>
Update website: rebuilt with latest changes
</commit_message>
<xml_diff>
--- a/Trial/osl18/Temp.xlsx
+++ b/Trial/osl18/Temp.xlsx
@@ -5,32 +5,44 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parth\Desktop\Trial\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3729f9cc1dcc55e0/WORK/Website/palclim/Trial/osl18/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49527EA0-A3C0-47B3-95B0-A747A3BC8B76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{49527EA0-A3C0-47B3-95B0-A747A3BC8B76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4BB82F32-7E14-40CB-8B09-4969016AACAB}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-1950" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Age [ka BP]</t>
   </si>
   <si>
     <t>Temp interp [°C]</t>
+  </si>
+  <si>
+    <t>Err</t>
   </si>
 </sst>
 </file>
@@ -348,2500 +360,3743 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B311"/>
+  <dimension ref="A1:C311"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C311"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>27.2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <f>B2*2/100</f>
+        <v>0.54400000000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>12.772</v>
       </c>
       <c r="B3">
         <v>27.2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3">
+        <f t="shared" ref="C3:C66" si="0">B3*2/100</f>
+        <v>0.54400000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>13.122999999999999</v>
       </c>
       <c r="B4">
         <v>26.4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>0.52800000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>13.677</v>
       </c>
       <c r="B5">
         <v>26.6</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>0.53200000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>13.769</v>
       </c>
       <c r="B6">
         <v>26.2</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>0.52400000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>13.944000000000001</v>
       </c>
       <c r="B7">
         <v>28.1</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>0.56200000000000006</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>14.029</v>
       </c>
       <c r="B8">
         <v>25.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>14.204000000000001</v>
       </c>
       <c r="B9">
         <v>26.8</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>0.53600000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>14.291</v>
       </c>
       <c r="B10">
         <v>25.6</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>0.51200000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>14.551</v>
       </c>
       <c r="B11">
         <v>26.1</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>0.52200000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>14.635999999999999</v>
       </c>
       <c r="B12">
         <v>26.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>14.723000000000001</v>
       </c>
       <c r="B13">
         <v>27.4</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>0.54799999999999993</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>14.808999999999999</v>
       </c>
       <c r="B14">
         <v>26.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14.981999999999999</v>
       </c>
       <c r="B15">
         <v>26</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15.068</v>
       </c>
       <c r="B16">
         <v>26.3</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>0.52600000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15.154999999999999</v>
       </c>
       <c r="B17">
         <v>25.8</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>0.51600000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>15.24</v>
       </c>
       <c r="B18">
         <v>26.8</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>0.53600000000000003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>15.327</v>
       </c>
       <c r="B19">
         <v>26.3</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>0.52600000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>15.414999999999999</v>
       </c>
       <c r="B20">
         <v>25.6</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>0.51200000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>15.500999999999999</v>
       </c>
       <c r="B21">
         <v>25.4</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>0.50800000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>15.587999999999999</v>
       </c>
       <c r="B22">
         <v>25.3</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>0.50600000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>15.673999999999999</v>
       </c>
       <c r="B23">
         <v>26.4</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>0.52800000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>15.760999999999999</v>
       </c>
       <c r="B24">
         <v>25.6</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>0.51200000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>15.85</v>
       </c>
       <c r="B25">
         <v>25.9</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>0.51800000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>15.935</v>
       </c>
       <c r="B26">
         <v>25.7</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>0.51400000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>16.021999999999998</v>
       </c>
       <c r="B27">
         <v>26.1</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>0.52200000000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>16.108000000000001</v>
       </c>
       <c r="B28">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>16.193999999999999</v>
       </c>
       <c r="B29">
         <v>25.8</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>0.51600000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>16.280999999999999</v>
       </c>
       <c r="B30">
         <v>25.7</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>0.51400000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>16.367000000000001</v>
       </c>
       <c r="B31">
         <v>26.2</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>0.52400000000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>16.451000000000001</v>
       </c>
       <c r="B32">
         <v>25.1</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>0.502</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>16.536000000000001</v>
       </c>
       <c r="B33">
         <v>25.3</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>0.50600000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>16.622</v>
       </c>
       <c r="B34">
         <v>24.2</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>0.48399999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>16.794</v>
       </c>
       <c r="B35">
         <v>27.1</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>0.54200000000000004</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>16.881</v>
       </c>
       <c r="B36">
         <v>25.5</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>16.968</v>
       </c>
       <c r="B37">
         <v>25.6</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>0.51200000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>17.053999999999998</v>
       </c>
       <c r="B38">
         <v>25.5</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>17.140999999999998</v>
       </c>
       <c r="B39">
         <v>26.4</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>0.52800000000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>17.227</v>
       </c>
       <c r="B40">
         <v>26.2</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>0.52400000000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>17.402000000000001</v>
       </c>
       <c r="B41">
         <v>25.1</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>0.502</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>17.571999999999999</v>
       </c>
       <c r="B42">
         <v>27</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>17.829999999999998</v>
       </c>
       <c r="B43">
         <v>25.8</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C43">
+        <f t="shared" si="0"/>
+        <v>0.51600000000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>17.914999999999999</v>
       </c>
       <c r="B44">
         <v>24.5</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C44">
+        <f t="shared" si="0"/>
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>18.001000000000001</v>
       </c>
       <c r="B45">
         <v>24.7</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>0.49399999999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>18.085999999999999</v>
       </c>
       <c r="B46">
         <v>23.5</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C46">
+        <f t="shared" si="0"/>
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>18.172999999999998</v>
       </c>
       <c r="B47">
         <v>24.1</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C47">
+        <f t="shared" si="0"/>
+        <v>0.48200000000000004</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>18.259</v>
       </c>
       <c r="B48">
         <v>23</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C48">
+        <f t="shared" si="0"/>
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>18.344999999999999</v>
       </c>
       <c r="B49">
         <v>24.6</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C49">
+        <f t="shared" si="0"/>
+        <v>0.49200000000000005</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>18.431000000000001</v>
       </c>
       <c r="B50">
         <v>24.8</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C50">
+        <f t="shared" si="0"/>
+        <v>0.496</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>18.516999999999999</v>
       </c>
       <c r="B51">
         <v>25.2</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C51">
+        <f t="shared" si="0"/>
+        <v>0.504</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>18.602</v>
       </c>
       <c r="B52">
         <v>25.3</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C52">
+        <f t="shared" si="0"/>
+        <v>0.50600000000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>18.689</v>
       </c>
       <c r="B53">
         <v>24.4</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C53">
+        <f t="shared" si="0"/>
+        <v>0.48799999999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>18.782</v>
       </c>
       <c r="B54">
         <v>24.2</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C54">
+        <f t="shared" si="0"/>
+        <v>0.48399999999999999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>18.879000000000001</v>
       </c>
       <c r="B55">
         <v>24.2</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C55">
+        <f t="shared" si="0"/>
+        <v>0.48399999999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>18.977</v>
       </c>
       <c r="B56">
         <v>23.7</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C56">
+        <f t="shared" si="0"/>
+        <v>0.47399999999999998</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>19.076000000000001</v>
       </c>
       <c r="B57">
         <v>24.2</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C57">
+        <f t="shared" si="0"/>
+        <v>0.48399999999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>19.173999999999999</v>
       </c>
       <c r="B58">
         <v>23.8</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C58">
+        <f t="shared" si="0"/>
+        <v>0.47600000000000003</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>19.271999999999998</v>
       </c>
       <c r="B59">
         <v>24.7</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C59">
+        <f t="shared" si="0"/>
+        <v>0.49399999999999999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>19.372</v>
       </c>
       <c r="B60">
         <v>24.7</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C60">
+        <f t="shared" si="0"/>
+        <v>0.49399999999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>19.471</v>
       </c>
       <c r="B61">
         <v>24.4</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C61">
+        <f t="shared" si="0"/>
+        <v>0.48799999999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>19.568999999999999</v>
       </c>
       <c r="B62">
         <v>24.2</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C62">
+        <f t="shared" si="0"/>
+        <v>0.48399999999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>19.666</v>
       </c>
       <c r="B63">
         <v>25.1</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C63">
+        <f t="shared" si="0"/>
+        <v>0.502</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>19.763999999999999</v>
       </c>
       <c r="B64">
         <v>24.4</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C64">
+        <f t="shared" si="0"/>
+        <v>0.48799999999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>19.863</v>
       </c>
       <c r="B65">
         <v>25</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C65">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>19.960999999999999</v>
       </c>
       <c r="B66">
         <v>24.4</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C66">
+        <f t="shared" si="0"/>
+        <v>0.48799999999999999</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>20.058</v>
       </c>
       <c r="B67">
         <v>24.2</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C67">
+        <f t="shared" ref="C67:C130" si="1">B67*2/100</f>
+        <v>0.48399999999999999</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>20.155999999999999</v>
       </c>
       <c r="B68">
         <v>24.8</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C68">
+        <f t="shared" si="1"/>
+        <v>0.496</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>20.251999999999999</v>
       </c>
       <c r="B69">
         <v>24.8</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C69">
+        <f t="shared" si="1"/>
+        <v>0.496</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>20.352</v>
       </c>
       <c r="B70">
         <v>24.3</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C70">
+        <f t="shared" si="1"/>
+        <v>0.48599999999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>20.451000000000001</v>
       </c>
       <c r="B71">
         <v>24.3</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C71">
+        <f t="shared" si="1"/>
+        <v>0.48599999999999999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>20.55</v>
       </c>
       <c r="B72">
         <v>24.7</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C72">
+        <f t="shared" si="1"/>
+        <v>0.49399999999999999</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>20.65</v>
       </c>
       <c r="B73">
         <v>24.1</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C73">
+        <f t="shared" si="1"/>
+        <v>0.48200000000000004</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>20.748000000000001</v>
       </c>
       <c r="B74">
         <v>24.1</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C74">
+        <f t="shared" si="1"/>
+        <v>0.48200000000000004</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>20.847000000000001</v>
       </c>
       <c r="B75">
         <v>24.9</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C75">
+        <f t="shared" si="1"/>
+        <v>0.498</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>20.946000000000002</v>
       </c>
       <c r="B76">
         <v>24.6</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C76">
+        <f t="shared" si="1"/>
+        <v>0.49200000000000005</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>21.042999999999999</v>
       </c>
       <c r="B77">
         <v>24.9</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C77">
+        <f t="shared" si="1"/>
+        <v>0.498</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>21.315999999999999</v>
       </c>
       <c r="B78">
         <v>24.9</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C78">
+        <f t="shared" si="1"/>
+        <v>0.498</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>21.399000000000001</v>
       </c>
       <c r="B79">
         <v>24.4</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C79">
+        <f t="shared" si="1"/>
+        <v>0.48799999999999999</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>21.486000000000001</v>
       </c>
       <c r="B80">
         <v>24.9</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C80">
+        <f t="shared" si="1"/>
+        <v>0.498</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>21.571999999999999</v>
       </c>
       <c r="B81">
         <v>24.3</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C81">
+        <f t="shared" si="1"/>
+        <v>0.48599999999999999</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>21.655000000000001</v>
       </c>
       <c r="B82">
         <v>24.4</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C82">
+        <f t="shared" si="1"/>
+        <v>0.48799999999999999</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>21.74</v>
       </c>
       <c r="B83">
         <v>24.5</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C83">
+        <f t="shared" si="1"/>
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>21.824000000000002</v>
       </c>
       <c r="B84">
         <v>24.6</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C84">
+        <f t="shared" si="1"/>
+        <v>0.49200000000000005</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>21.91</v>
       </c>
       <c r="B85">
         <v>25</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C85">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>21.995000000000001</v>
       </c>
       <c r="B86">
         <v>24.7</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C86">
+        <f t="shared" si="1"/>
+        <v>0.49399999999999999</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>22.164999999999999</v>
       </c>
       <c r="B87">
         <v>24.2</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C87">
+        <f t="shared" si="1"/>
+        <v>0.48399999999999999</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>22.337</v>
       </c>
       <c r="B88">
         <v>24.7</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C88">
+        <f t="shared" si="1"/>
+        <v>0.49399999999999999</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>22.425000000000001</v>
       </c>
       <c r="B89">
         <v>24.5</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C89">
+        <f t="shared" si="1"/>
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>22.510999999999999</v>
       </c>
       <c r="B90">
         <v>24.2</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C90">
+        <f t="shared" si="1"/>
+        <v>0.48399999999999999</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>22.597000000000001</v>
       </c>
       <c r="B91">
         <v>24.9</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C91">
+        <f t="shared" si="1"/>
+        <v>0.498</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>22.681000000000001</v>
       </c>
       <c r="B92">
         <v>23.9</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C92">
+        <f t="shared" si="1"/>
+        <v>0.47799999999999998</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>22.766999999999999</v>
       </c>
       <c r="B93">
         <v>24</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C93">
+        <f t="shared" si="1"/>
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>22.850999999999999</v>
       </c>
       <c r="B94">
         <v>23.6</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C94">
+        <f t="shared" si="1"/>
+        <v>0.47200000000000003</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>22.936</v>
       </c>
       <c r="B95">
         <v>23.8</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C95">
+        <f t="shared" si="1"/>
+        <v>0.47600000000000003</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>23.021999999999998</v>
       </c>
       <c r="B96">
         <v>23.4</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C96">
+        <f t="shared" si="1"/>
+        <v>0.46799999999999997</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>23.108000000000001</v>
       </c>
       <c r="B97">
         <v>24.2</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C97">
+        <f t="shared" si="1"/>
+        <v>0.48399999999999999</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>23.196000000000002</v>
       </c>
       <c r="B98">
         <v>24.1</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C98">
+        <f t="shared" si="1"/>
+        <v>0.48200000000000004</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>23.283999999999999</v>
       </c>
       <c r="B99">
         <v>23.4</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C99">
+        <f t="shared" si="1"/>
+        <v>0.46799999999999997</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>23.376000000000001</v>
       </c>
       <c r="B100">
         <v>24.5</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C100">
+        <f t="shared" si="1"/>
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>23.472999999999999</v>
       </c>
       <c r="B101">
         <v>24.5</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C101">
+        <f t="shared" si="1"/>
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>23.57</v>
       </c>
       <c r="B102">
         <v>24.8</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C102">
+        <f t="shared" si="1"/>
+        <v>0.496</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>23.666</v>
       </c>
       <c r="B103">
         <v>24.5</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C103">
+        <f t="shared" si="1"/>
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>23.763000000000002</v>
       </c>
       <c r="B104">
         <v>24.7</v>
       </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C104">
+        <f t="shared" si="1"/>
+        <v>0.49399999999999999</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>23.86</v>
       </c>
       <c r="B105">
         <v>25</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C105">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>23.957999999999998</v>
       </c>
       <c r="B106">
         <v>24.5</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C106">
+        <f t="shared" si="1"/>
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>24.056000000000001</v>
       </c>
       <c r="B107">
         <v>24.6</v>
       </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C107">
+        <f t="shared" si="1"/>
+        <v>0.49200000000000005</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>24.25</v>
       </c>
       <c r="B108">
         <v>25.4</v>
       </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C108">
+        <f t="shared" si="1"/>
+        <v>0.50800000000000001</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>24.344999999999999</v>
       </c>
       <c r="B109">
         <v>26.1</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C109">
+        <f t="shared" si="1"/>
+        <v>0.52200000000000002</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>24.439</v>
       </c>
       <c r="B110">
         <v>24.7</v>
       </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C110">
+        <f t="shared" si="1"/>
+        <v>0.49399999999999999</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>24.535</v>
       </c>
       <c r="B111">
         <v>25.3</v>
       </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C111">
+        <f t="shared" si="1"/>
+        <v>0.50600000000000001</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>24.632000000000001</v>
       </c>
       <c r="B112">
         <v>24.6</v>
       </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C112">
+        <f t="shared" si="1"/>
+        <v>0.49200000000000005</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>24.728999999999999</v>
       </c>
       <c r="B113">
         <v>24.9</v>
       </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C113">
+        <f t="shared" si="1"/>
+        <v>0.498</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>24.824999999999999</v>
       </c>
       <c r="B114">
         <v>25.1</v>
       </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C114">
+        <f t="shared" si="1"/>
+        <v>0.502</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>24.920999999999999</v>
       </c>
       <c r="B115">
         <v>24.8</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C115">
+        <f t="shared" si="1"/>
+        <v>0.496</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>25.018000000000001</v>
       </c>
       <c r="B116">
         <v>24.9</v>
       </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C116">
+        <f t="shared" si="1"/>
+        <v>0.498</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>25.114999999999998</v>
       </c>
       <c r="B117">
         <v>25.1</v>
       </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C117">
+        <f t="shared" si="1"/>
+        <v>0.502</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>25.212</v>
       </c>
       <c r="B118">
         <v>24.5</v>
       </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C118">
+        <f t="shared" si="1"/>
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>25.309000000000001</v>
       </c>
       <c r="B119">
         <v>26</v>
       </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C119">
+        <f t="shared" si="1"/>
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>25.404</v>
       </c>
       <c r="B120">
         <v>25.3</v>
       </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C120">
+        <f t="shared" si="1"/>
+        <v>0.50600000000000001</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>25.498999999999999</v>
       </c>
       <c r="B121">
         <v>25</v>
       </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C121">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>25.591999999999999</v>
       </c>
       <c r="B122">
         <v>25.3</v>
       </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C122">
+        <f t="shared" si="1"/>
+        <v>0.50600000000000001</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>25.687000000000001</v>
       </c>
       <c r="B123">
         <v>25.2</v>
       </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C123">
+        <f t="shared" si="1"/>
+        <v>0.504</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>25.777000000000001</v>
       </c>
       <c r="B124">
         <v>25.8</v>
       </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C124">
+        <f t="shared" si="1"/>
+        <v>0.51600000000000001</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>25.863</v>
       </c>
       <c r="B125">
         <v>25.2</v>
       </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C125">
+        <f t="shared" si="1"/>
+        <v>0.504</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>25.949000000000002</v>
       </c>
       <c r="B126">
         <v>25.4</v>
       </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C126">
+        <f t="shared" si="1"/>
+        <v>0.50800000000000001</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>26.036000000000001</v>
       </c>
       <c r="B127">
         <v>25.6</v>
       </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C127">
+        <f t="shared" si="1"/>
+        <v>0.51200000000000001</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>26.122</v>
       </c>
       <c r="B128">
         <v>25.4</v>
       </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C128">
+        <f t="shared" si="1"/>
+        <v>0.50800000000000001</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>26.206</v>
       </c>
       <c r="B129">
         <v>24.2</v>
       </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C129">
+        <f t="shared" si="1"/>
+        <v>0.48399999999999999</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>26.288</v>
       </c>
       <c r="B130">
         <v>24.9</v>
       </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C130">
+        <f t="shared" si="1"/>
+        <v>0.498</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>26.370999999999999</v>
       </c>
       <c r="B131">
         <v>24.8</v>
       </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C131">
+        <f t="shared" ref="C131:C194" si="2">B131*2/100</f>
+        <v>0.496</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>26.457000000000001</v>
       </c>
       <c r="B132">
         <v>25.1</v>
       </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C132">
+        <f t="shared" si="2"/>
+        <v>0.502</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>26.544</v>
       </c>
       <c r="B133">
         <v>24.6</v>
       </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C133">
+        <f t="shared" si="2"/>
+        <v>0.49200000000000005</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>26.629000000000001</v>
       </c>
       <c r="B134">
         <v>24.5</v>
       </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C134">
+        <f t="shared" si="2"/>
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>26.800999999999998</v>
       </c>
       <c r="B135">
         <v>24.3</v>
       </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C135">
+        <f t="shared" si="2"/>
+        <v>0.48599999999999999</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>26.885999999999999</v>
       </c>
       <c r="B136">
         <v>24.4</v>
       </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C136">
+        <f t="shared" si="2"/>
+        <v>0.48799999999999999</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>26.972999999999999</v>
       </c>
       <c r="B137">
         <v>24.4</v>
       </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C137">
+        <f t="shared" si="2"/>
+        <v>0.48799999999999999</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>27.059000000000001</v>
       </c>
       <c r="B138">
         <v>24.4</v>
       </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C138">
+        <f t="shared" si="2"/>
+        <v>0.48799999999999999</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>27.145</v>
       </c>
       <c r="B139">
         <v>24.7</v>
       </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C139">
+        <f t="shared" si="2"/>
+        <v>0.49399999999999999</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>27.231999999999999</v>
       </c>
       <c r="B140">
         <v>25.4</v>
       </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C140">
+        <f t="shared" si="2"/>
+        <v>0.50800000000000001</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>27.317</v>
       </c>
       <c r="B141">
         <v>24.7</v>
       </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C141">
+        <f t="shared" si="2"/>
+        <v>0.49399999999999999</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>27.402000000000001</v>
       </c>
       <c r="B142">
         <v>25</v>
       </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C142">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>27.488</v>
       </c>
       <c r="B143">
         <v>25</v>
       </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C143">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>27.573</v>
       </c>
       <c r="B144">
         <v>24.9</v>
       </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C144">
+        <f t="shared" si="2"/>
+        <v>0.498</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>27.658999999999999</v>
       </c>
       <c r="B145">
         <v>24.8</v>
       </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C145">
+        <f t="shared" si="2"/>
+        <v>0.496</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>27.748000000000001</v>
       </c>
       <c r="B146">
         <v>24.9</v>
       </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C146">
+        <f t="shared" si="2"/>
+        <v>0.498</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>27.937999999999999</v>
       </c>
       <c r="B147">
         <v>24.3</v>
       </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C147">
+        <f t="shared" si="2"/>
+        <v>0.48599999999999999</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>28.056000000000001</v>
       </c>
       <c r="B148">
         <v>25.4</v>
       </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C148">
+        <f t="shared" si="2"/>
+        <v>0.50800000000000001</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>28.172999999999998</v>
       </c>
       <c r="B149">
         <v>25.1</v>
       </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C149">
+        <f t="shared" si="2"/>
+        <v>0.502</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>28.29</v>
       </c>
       <c r="B150">
         <v>24.7</v>
       </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C150">
+        <f t="shared" si="2"/>
+        <v>0.49399999999999999</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>28.408999999999999</v>
       </c>
       <c r="B151">
         <v>24.9</v>
       </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C151">
+        <f t="shared" si="2"/>
+        <v>0.498</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>28.527000000000001</v>
       </c>
       <c r="B152">
         <v>24.7</v>
       </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C152">
+        <f t="shared" si="2"/>
+        <v>0.49399999999999999</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>28.646999999999998</v>
       </c>
       <c r="B153">
         <v>25</v>
       </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C153">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>28.765000000000001</v>
       </c>
       <c r="B154">
         <v>24.6</v>
       </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C154">
+        <f t="shared" si="2"/>
+        <v>0.49200000000000005</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>28.884</v>
       </c>
       <c r="B155">
         <v>25.5</v>
       </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C155">
+        <f t="shared" si="2"/>
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>29.003</v>
       </c>
       <c r="B156">
         <v>25.2</v>
       </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C156">
+        <f t="shared" si="2"/>
+        <v>0.504</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>29.122</v>
       </c>
       <c r="B157">
         <v>25.7</v>
       </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C157">
+        <f t="shared" si="2"/>
+        <v>0.51400000000000001</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>29.24</v>
       </c>
       <c r="B158">
         <v>25.2</v>
       </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C158">
+        <f t="shared" si="2"/>
+        <v>0.504</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>29.36</v>
       </c>
       <c r="B159">
         <v>25.8</v>
       </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C159">
+        <f t="shared" si="2"/>
+        <v>0.51600000000000001</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>29.478000000000002</v>
       </c>
       <c r="B160">
         <v>25.5</v>
       </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C160">
+        <f t="shared" si="2"/>
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>29.597000000000001</v>
       </c>
       <c r="B161">
         <v>26.6</v>
       </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C161">
+        <f t="shared" si="2"/>
+        <v>0.53200000000000003</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>29.712</v>
       </c>
       <c r="B162">
         <v>26.5</v>
       </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C162">
+        <f t="shared" si="2"/>
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>29.831</v>
       </c>
       <c r="B163">
         <v>25.7</v>
       </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C163">
+        <f t="shared" si="2"/>
+        <v>0.51400000000000001</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>29.95</v>
       </c>
       <c r="B164">
         <v>25.5</v>
       </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C164">
+        <f t="shared" si="2"/>
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>30.064</v>
       </c>
       <c r="B165">
         <v>25.7</v>
       </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C165">
+        <f t="shared" si="2"/>
+        <v>0.51400000000000001</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>30.18</v>
       </c>
       <c r="B166">
         <v>24.6</v>
       </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C166">
+        <f t="shared" si="2"/>
+        <v>0.49200000000000005</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>30.295999999999999</v>
       </c>
       <c r="B167">
         <v>24.5</v>
       </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C167">
+        <f t="shared" si="2"/>
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>30.414999999999999</v>
       </c>
       <c r="B168">
         <v>25.6</v>
       </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C168">
+        <f t="shared" si="2"/>
+        <v>0.51200000000000001</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>30.533000000000001</v>
       </c>
       <c r="B169">
         <v>25.1</v>
       </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C169">
+        <f t="shared" si="2"/>
+        <v>0.502</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>30.652999999999999</v>
       </c>
       <c r="B170">
         <v>24.9</v>
       </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C170">
+        <f t="shared" si="2"/>
+        <v>0.498</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>30.774000000000001</v>
       </c>
       <c r="B171">
         <v>24.6</v>
       </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C171">
+        <f t="shared" si="2"/>
+        <v>0.49200000000000005</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>30.893000000000001</v>
       </c>
       <c r="B172">
         <v>24.7</v>
       </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C172">
+        <f t="shared" si="2"/>
+        <v>0.49399999999999999</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>31.009</v>
       </c>
       <c r="B173">
         <v>25.3</v>
       </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C173">
+        <f t="shared" si="2"/>
+        <v>0.50600000000000001</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>31.128</v>
       </c>
       <c r="B174">
         <v>25.2</v>
       </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C174">
+        <f t="shared" si="2"/>
+        <v>0.504</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>31.244</v>
       </c>
       <c r="B175">
         <v>24.7</v>
       </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C175">
+        <f t="shared" si="2"/>
+        <v>0.49399999999999999</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>31.361000000000001</v>
       </c>
       <c r="B176">
         <v>25</v>
       </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C176">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>31.475999999999999</v>
       </c>
       <c r="B177">
         <v>25.7</v>
       </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C177">
+        <f t="shared" si="2"/>
+        <v>0.51400000000000001</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>31.594000000000001</v>
       </c>
       <c r="B178">
         <v>25.1</v>
       </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C178">
+        <f t="shared" si="2"/>
+        <v>0.502</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>31.713000000000001</v>
       </c>
       <c r="B179">
         <v>25.2</v>
       </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C179">
+        <f t="shared" si="2"/>
+        <v>0.504</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>31.831</v>
       </c>
       <c r="B180">
         <v>25.3</v>
       </c>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C180">
+        <f t="shared" si="2"/>
+        <v>0.50600000000000001</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>31.948</v>
       </c>
       <c r="B181">
         <v>24.8</v>
       </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C181">
+        <f t="shared" si="2"/>
+        <v>0.496</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>32.064</v>
       </c>
       <c r="B182">
         <v>23.8</v>
       </c>
-    </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C182">
+        <f t="shared" si="2"/>
+        <v>0.47600000000000003</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>32.298000000000002</v>
       </c>
       <c r="B183">
         <v>25</v>
       </c>
-    </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C183">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>32.415999999999997</v>
       </c>
       <c r="B184">
         <v>24.7</v>
       </c>
-    </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C184">
+        <f t="shared" si="2"/>
+        <v>0.49399999999999999</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>32.533999999999999</v>
       </c>
       <c r="B185">
         <v>24.7</v>
       </c>
-    </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C185">
+        <f t="shared" si="2"/>
+        <v>0.49399999999999999</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>32.652000000000001</v>
       </c>
       <c r="B186">
         <v>24.2</v>
       </c>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C186">
+        <f t="shared" si="2"/>
+        <v>0.48399999999999999</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>32.889000000000003</v>
       </c>
       <c r="B187">
         <v>25.6</v>
       </c>
-    </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C187">
+        <f t="shared" si="2"/>
+        <v>0.51200000000000001</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>33.005000000000003</v>
       </c>
       <c r="B188">
         <v>25.5</v>
       </c>
-    </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C188">
+        <f t="shared" si="2"/>
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>33.122</v>
       </c>
       <c r="B189">
         <v>25.1</v>
       </c>
-    </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C189">
+        <f t="shared" si="2"/>
+        <v>0.502</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>33.238999999999997</v>
       </c>
       <c r="B190">
         <v>25</v>
       </c>
-    </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C190">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>33.356999999999999</v>
       </c>
       <c r="B191">
         <v>24.8</v>
       </c>
-    </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C191">
+        <f t="shared" si="2"/>
+        <v>0.496</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>33.475999999999999</v>
       </c>
       <c r="B192">
         <v>25</v>
       </c>
-    </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C192">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>33.593000000000004</v>
       </c>
       <c r="B193">
         <v>25.5</v>
       </c>
-    </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C193">
+        <f t="shared" si="2"/>
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>33.709000000000003</v>
       </c>
       <c r="B194">
         <v>25.2</v>
       </c>
-    </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C194">
+        <f t="shared" si="2"/>
+        <v>0.504</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>33.817</v>
       </c>
       <c r="B195">
         <v>24.2</v>
       </c>
-    </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C195">
+        <f t="shared" ref="C195:C258" si="3">B195*2/100</f>
+        <v>0.48399999999999999</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>34.020000000000003</v>
       </c>
       <c r="B196">
         <v>25.5</v>
       </c>
-    </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C196">
+        <f t="shared" si="3"/>
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>34.121000000000002</v>
       </c>
       <c r="B197">
         <v>25.5</v>
       </c>
-    </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C197">
+        <f t="shared" si="3"/>
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>34.222999999999999</v>
       </c>
       <c r="B198">
         <v>25.8</v>
       </c>
-    </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C198">
+        <f t="shared" si="3"/>
+        <v>0.51600000000000001</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>34.323999999999998</v>
       </c>
       <c r="B199">
         <v>26</v>
       </c>
-    </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C199">
+        <f t="shared" si="3"/>
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>34.427999999999997</v>
       </c>
       <c r="B200">
         <v>25.5</v>
       </c>
-    </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C200">
+        <f t="shared" si="3"/>
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>34.530999999999999</v>
       </c>
       <c r="B201">
         <v>24.9</v>
       </c>
-    </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C201">
+        <f t="shared" si="3"/>
+        <v>0.498</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>34.633000000000003</v>
       </c>
       <c r="B202">
         <v>25.6</v>
       </c>
-    </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C202">
+        <f t="shared" si="3"/>
+        <v>0.51200000000000001</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>34.734000000000002</v>
       </c>
       <c r="B203">
         <v>24.9</v>
       </c>
-    </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C203">
+        <f t="shared" si="3"/>
+        <v>0.498</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>34.834000000000003</v>
       </c>
       <c r="B204">
         <v>24.4</v>
       </c>
-    </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C204">
+        <f t="shared" si="3"/>
+        <v>0.48799999999999999</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>34.936999999999998</v>
       </c>
       <c r="B205">
         <v>25</v>
       </c>
-    </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C205">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>35.039000000000001</v>
       </c>
       <c r="B206">
         <v>24.9</v>
       </c>
-    </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C206">
+        <f t="shared" si="3"/>
+        <v>0.498</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>35.14</v>
       </c>
       <c r="B207">
         <v>25.2</v>
       </c>
-    </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C207">
+        <f t="shared" si="3"/>
+        <v>0.504</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>35.243000000000002</v>
       </c>
       <c r="B208">
         <v>25</v>
       </c>
-    </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C208">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>35.344000000000001</v>
       </c>
       <c r="B209">
         <v>25.2</v>
       </c>
-    </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C209">
+        <f t="shared" si="3"/>
+        <v>0.504</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>35.445999999999998</v>
       </c>
       <c r="B210">
         <v>26.4</v>
       </c>
-    </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C210">
+        <f t="shared" si="3"/>
+        <v>0.52800000000000002</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>35.545000000000002</v>
       </c>
       <c r="B211">
         <v>26.6</v>
       </c>
-    </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C211">
+        <f t="shared" si="3"/>
+        <v>0.53200000000000003</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>35.65</v>
       </c>
       <c r="B212">
         <v>25.7</v>
       </c>
-    </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C212">
+        <f t="shared" si="3"/>
+        <v>0.51400000000000001</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>35.755000000000003</v>
       </c>
       <c r="B213">
         <v>24.5</v>
       </c>
-    </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C213">
+        <f t="shared" si="3"/>
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>35.859000000000002</v>
       </c>
       <c r="B214">
         <v>25</v>
       </c>
-    </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C214">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>35.962000000000003</v>
       </c>
       <c r="B215">
         <v>25.9</v>
       </c>
-    </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C215">
+        <f t="shared" si="3"/>
+        <v>0.51800000000000002</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>36.064</v>
       </c>
       <c r="B216">
         <v>25.4</v>
       </c>
-    </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C216">
+        <f t="shared" si="3"/>
+        <v>0.50800000000000001</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>36.17</v>
       </c>
       <c r="B217">
         <v>24.3</v>
       </c>
-    </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C217">
+        <f t="shared" si="3"/>
+        <v>0.48599999999999999</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>36.274999999999999</v>
       </c>
       <c r="B218">
         <v>25.3</v>
       </c>
-    </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C218">
+        <f t="shared" si="3"/>
+        <v>0.50600000000000001</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>36.405999999999999</v>
       </c>
       <c r="B219">
         <v>25.5</v>
       </c>
-    </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C219">
+        <f t="shared" si="3"/>
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>36.56</v>
       </c>
       <c r="B220">
         <v>24.9</v>
       </c>
-    </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C220">
+        <f t="shared" si="3"/>
+        <v>0.498</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>36.715000000000003</v>
       </c>
       <c r="B221">
         <v>25.4</v>
       </c>
-    </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C221">
+        <f t="shared" si="3"/>
+        <v>0.50800000000000001</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>36.872</v>
       </c>
       <c r="B222">
         <v>26.1</v>
       </c>
-    </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C222">
+        <f t="shared" si="3"/>
+        <v>0.52200000000000002</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>37.027999999999999</v>
       </c>
       <c r="B223">
         <v>24.9</v>
       </c>
-    </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C223">
+        <f t="shared" si="3"/>
+        <v>0.498</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>37.185000000000002</v>
       </c>
       <c r="B224">
         <v>24.7</v>
       </c>
-    </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C224">
+        <f t="shared" si="3"/>
+        <v>0.49399999999999999</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>37.341000000000001</v>
       </c>
       <c r="B225">
         <v>25.3</v>
       </c>
-    </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C225">
+        <f t="shared" si="3"/>
+        <v>0.50600000000000001</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>37.496000000000002</v>
       </c>
       <c r="B226">
         <v>24.7</v>
       </c>
-    </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C226">
+        <f t="shared" si="3"/>
+        <v>0.49399999999999999</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>37.654000000000003</v>
       </c>
       <c r="B227">
         <v>25.7</v>
       </c>
-    </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C227">
+        <f t="shared" si="3"/>
+        <v>0.51400000000000001</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>37.811</v>
       </c>
       <c r="B228">
         <v>25.9</v>
       </c>
-    </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C228">
+        <f t="shared" si="3"/>
+        <v>0.51800000000000002</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>37.966999999999999</v>
       </c>
       <c r="B229">
         <v>25.3</v>
       </c>
-    </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C229">
+        <f t="shared" si="3"/>
+        <v>0.50600000000000001</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>38.281999999999996</v>
       </c>
       <c r="B230">
         <v>27</v>
       </c>
-    </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C230">
+        <f t="shared" si="3"/>
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>38.435000000000002</v>
       </c>
       <c r="B231">
         <v>27.1</v>
       </c>
-    </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C231">
+        <f t="shared" si="3"/>
+        <v>0.54200000000000004</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>38.588999999999999</v>
       </c>
       <c r="B232">
         <v>26.9</v>
       </c>
-    </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C232">
+        <f t="shared" si="3"/>
+        <v>0.53799999999999992</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>38.744999999999997</v>
       </c>
       <c r="B233">
         <v>26.5</v>
       </c>
-    </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C233">
+        <f t="shared" si="3"/>
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>38.902000000000001</v>
       </c>
       <c r="B234">
         <v>25.7</v>
       </c>
-    </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C234">
+        <f t="shared" si="3"/>
+        <v>0.51400000000000001</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>39.061</v>
       </c>
       <c r="B235">
         <v>26.4</v>
       </c>
-    </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C235">
+        <f t="shared" si="3"/>
+        <v>0.52800000000000002</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>39.215000000000003</v>
       </c>
       <c r="B236">
         <v>26.7</v>
       </c>
-    </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C236">
+        <f t="shared" si="3"/>
+        <v>0.53400000000000003</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>39.369</v>
       </c>
       <c r="B237">
         <v>25.6</v>
       </c>
-    </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C237">
+        <f t="shared" si="3"/>
+        <v>0.51200000000000001</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>39.524000000000001</v>
       </c>
       <c r="B238">
         <v>25.7</v>
       </c>
-    </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C238">
+        <f t="shared" si="3"/>
+        <v>0.51400000000000001</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>39.68</v>
       </c>
       <c r="B239">
         <v>26</v>
       </c>
-    </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C239">
+        <f t="shared" si="3"/>
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>39.835000000000001</v>
       </c>
       <c r="B240">
         <v>25.9</v>
       </c>
-    </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C240">
+        <f t="shared" si="3"/>
+        <v>0.51800000000000002</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>40.140999999999998</v>
       </c>
       <c r="B241">
         <v>26.1</v>
       </c>
-    </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C241">
+        <f t="shared" si="3"/>
+        <v>0.52200000000000002</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>40.276000000000003</v>
       </c>
       <c r="B242">
         <v>25.4</v>
       </c>
-    </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C242">
+        <f t="shared" si="3"/>
+        <v>0.50800000000000001</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>40.390999999999998</v>
       </c>
       <c r="B243">
         <v>25</v>
       </c>
-    </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C243">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>40.506999999999998</v>
       </c>
       <c r="B244">
         <v>24.4</v>
       </c>
-    </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C244">
+        <f t="shared" si="3"/>
+        <v>0.48799999999999999</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>40.622</v>
       </c>
       <c r="B245">
         <v>25.7</v>
       </c>
-    </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C245">
+        <f t="shared" si="3"/>
+        <v>0.51400000000000001</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>40.731999999999999</v>
       </c>
       <c r="B246">
         <v>24.5</v>
       </c>
-    </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C246">
+        <f t="shared" si="3"/>
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>40.844999999999999</v>
       </c>
       <c r="B247">
         <v>24.6</v>
       </c>
-    </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C247">
+        <f t="shared" si="3"/>
+        <v>0.49200000000000005</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>40.96</v>
       </c>
       <c r="B248">
         <v>24.7</v>
       </c>
-    </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C248">
+        <f t="shared" si="3"/>
+        <v>0.49399999999999999</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>41.076000000000001</v>
       </c>
       <c r="B249">
         <v>26.1</v>
       </c>
-    </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C249">
+        <f t="shared" si="3"/>
+        <v>0.52200000000000002</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>41.19</v>
       </c>
       <c r="B250">
         <v>25.5</v>
       </c>
-    </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C250">
+        <f t="shared" si="3"/>
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>41.305999999999997</v>
       </c>
       <c r="B251">
         <v>25.5</v>
       </c>
-    </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C251">
+        <f t="shared" si="3"/>
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>41.423000000000002</v>
       </c>
       <c r="B252">
         <v>25.3</v>
       </c>
-    </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C252">
+        <f t="shared" si="3"/>
+        <v>0.50600000000000001</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A253">
         <v>41.537999999999997</v>
       </c>
       <c r="B253">
         <v>25.1</v>
       </c>
-    </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C253">
+        <f t="shared" si="3"/>
+        <v>0.502</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A254">
         <v>41.65</v>
       </c>
       <c r="B254">
         <v>25.2</v>
       </c>
-    </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C254">
+        <f t="shared" si="3"/>
+        <v>0.504</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A255">
         <v>41.765999999999998</v>
       </c>
       <c r="B255">
         <v>24.6</v>
       </c>
-    </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C255">
+        <f t="shared" si="3"/>
+        <v>0.49200000000000005</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A256">
         <v>41.881999999999998</v>
       </c>
       <c r="B256">
         <v>23.9</v>
       </c>
-    </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C256">
+        <f t="shared" si="3"/>
+        <v>0.47799999999999998</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A257">
         <v>41.999000000000002</v>
       </c>
       <c r="B257">
         <v>24.6</v>
       </c>
-    </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C257">
+        <f t="shared" si="3"/>
+        <v>0.49200000000000005</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A258">
         <v>42.115000000000002</v>
       </c>
       <c r="B258">
         <v>24.9</v>
       </c>
-    </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C258">
+        <f t="shared" si="3"/>
+        <v>0.498</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A259">
         <v>42.231000000000002</v>
       </c>
       <c r="B259">
         <v>25.6</v>
       </c>
-    </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C259">
+        <f t="shared" ref="C259:C311" si="4">B259*2/100</f>
+        <v>0.51200000000000001</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A260">
         <v>42.347999999999999</v>
       </c>
       <c r="B260">
         <v>26.2</v>
       </c>
-    </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C260">
+        <f t="shared" si="4"/>
+        <v>0.52400000000000002</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A261">
         <v>42.463999999999999</v>
       </c>
       <c r="B261">
         <v>25.9</v>
       </c>
-    </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C261">
+        <f t="shared" si="4"/>
+        <v>0.51800000000000002</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A262">
         <v>42.581000000000003</v>
       </c>
       <c r="B262">
         <v>25.6</v>
       </c>
-    </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C262">
+        <f t="shared" si="4"/>
+        <v>0.51200000000000001</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A263">
         <v>42.697000000000003</v>
       </c>
       <c r="B263">
         <v>25.6</v>
       </c>
-    </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C263">
+        <f t="shared" si="4"/>
+        <v>0.51200000000000001</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A264">
         <v>42.813000000000002</v>
       </c>
       <c r="B264">
         <v>25.1</v>
       </c>
-    </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C264">
+        <f t="shared" si="4"/>
+        <v>0.502</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A265">
         <v>42.93</v>
       </c>
       <c r="B265">
         <v>26.3</v>
       </c>
-    </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C265">
+        <f t="shared" si="4"/>
+        <v>0.52600000000000002</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A266">
         <v>43.045999999999999</v>
       </c>
       <c r="B266">
         <v>25</v>
       </c>
-    </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C266">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A267">
         <v>43.161999999999999</v>
       </c>
       <c r="B267">
         <v>25.8</v>
       </c>
-    </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C267">
+        <f t="shared" si="4"/>
+        <v>0.51600000000000001</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A268">
         <v>43.28</v>
       </c>
       <c r="B268">
         <v>24.8</v>
       </c>
-    </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C268">
+        <f t="shared" si="4"/>
+        <v>0.496</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A269">
         <v>43.396999999999998</v>
       </c>
       <c r="B269">
         <v>25.9</v>
       </c>
-    </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C269">
+        <f t="shared" si="4"/>
+        <v>0.51800000000000002</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A270">
         <v>43.512999999999998</v>
       </c>
       <c r="B270">
         <v>26</v>
       </c>
-    </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C270">
+        <f t="shared" si="4"/>
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A271">
         <v>43.628</v>
       </c>
       <c r="B271">
         <v>25.8</v>
       </c>
-    </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C271">
+        <f t="shared" si="4"/>
+        <v>0.51600000000000001</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A272">
         <v>43.856999999999999</v>
       </c>
       <c r="B272">
         <v>25.6</v>
       </c>
-    </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C272">
+        <f t="shared" si="4"/>
+        <v>0.51200000000000001</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A273">
         <v>43.972000000000001</v>
       </c>
       <c r="B273">
         <v>25.5</v>
       </c>
-    </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C273">
+        <f t="shared" si="4"/>
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A274">
         <v>44.087000000000003</v>
       </c>
       <c r="B274">
         <v>25.3</v>
       </c>
-    </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C274">
+        <f t="shared" si="4"/>
+        <v>0.50600000000000001</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A275">
         <v>44.201000000000001</v>
       </c>
       <c r="B275">
         <v>24.6</v>
       </c>
-    </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C275">
+        <f t="shared" si="4"/>
+        <v>0.49200000000000005</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A276">
         <v>44.317</v>
       </c>
       <c r="B276">
         <v>25.8</v>
       </c>
-    </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C276">
+        <f t="shared" si="4"/>
+        <v>0.51600000000000001</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A277">
         <v>44.375</v>
       </c>
       <c r="B277">
         <v>25.6</v>
       </c>
-    </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C277">
+        <f t="shared" si="4"/>
+        <v>0.51200000000000001</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A278">
         <v>44.548999999999999</v>
       </c>
       <c r="B278">
         <v>25.6</v>
       </c>
-    </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C278">
+        <f t="shared" si="4"/>
+        <v>0.51200000000000001</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A279">
         <v>44.664999999999999</v>
       </c>
       <c r="B279">
         <v>25.1</v>
       </c>
-    </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C279">
+        <f t="shared" si="4"/>
+        <v>0.502</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A280">
         <v>44.781999999999996</v>
       </c>
       <c r="B280">
         <v>25.2</v>
       </c>
-    </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C280">
+        <f t="shared" si="4"/>
+        <v>0.504</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A281">
         <v>44.898000000000003</v>
       </c>
       <c r="B281">
         <v>24.5</v>
       </c>
-    </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C281">
+        <f t="shared" si="4"/>
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A282">
         <v>45.014000000000003</v>
       </c>
       <c r="B282">
         <v>24.5</v>
       </c>
-    </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C282">
+        <f t="shared" si="4"/>
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A283">
         <v>45.128999999999998</v>
       </c>
       <c r="B283">
         <v>25.4</v>
       </c>
-    </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C283">
+        <f t="shared" si="4"/>
+        <v>0.50800000000000001</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A284">
         <v>45.244</v>
       </c>
       <c r="B284">
         <v>24.9</v>
       </c>
-    </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C284">
+        <f t="shared" si="4"/>
+        <v>0.498</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A285">
         <v>45.357999999999997</v>
       </c>
       <c r="B285">
         <v>25</v>
       </c>
-    </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C285">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A286">
         <v>45.472000000000001</v>
       </c>
       <c r="B286">
         <v>25</v>
       </c>
-    </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C286">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A287">
         <v>45.585999999999999</v>
       </c>
       <c r="B287">
         <v>25.4</v>
       </c>
-    </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C287">
+        <f t="shared" si="4"/>
+        <v>0.50800000000000001</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A288">
         <v>45.7</v>
       </c>
       <c r="B288">
         <v>24.7</v>
       </c>
-    </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C288">
+        <f t="shared" si="4"/>
+        <v>0.49399999999999999</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A289">
         <v>45.813000000000002</v>
       </c>
       <c r="B289">
         <v>25.9</v>
       </c>
-    </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C289">
+        <f t="shared" si="4"/>
+        <v>0.51800000000000002</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A290">
         <v>45.926000000000002</v>
       </c>
       <c r="B290">
         <v>24.9</v>
       </c>
-    </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C290">
+        <f t="shared" si="4"/>
+        <v>0.498</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A291">
         <v>46.040999999999997</v>
       </c>
       <c r="B291">
         <v>25.3</v>
       </c>
-    </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C291">
+        <f t="shared" si="4"/>
+        <v>0.50600000000000001</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A292">
         <v>46.156999999999996</v>
       </c>
       <c r="B292">
         <v>25.6</v>
       </c>
-    </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C292">
+        <f t="shared" si="4"/>
+        <v>0.51200000000000001</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A293">
         <v>46.273000000000003</v>
       </c>
       <c r="B293">
         <v>26.2</v>
       </c>
-    </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C293">
+        <f t="shared" si="4"/>
+        <v>0.52400000000000002</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A294">
         <v>46.387999999999998</v>
       </c>
       <c r="B294">
         <v>27</v>
       </c>
-    </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C294">
+        <f t="shared" si="4"/>
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A295">
         <v>46.503</v>
       </c>
       <c r="B295">
         <v>26.1</v>
       </c>
-    </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C295">
+        <f t="shared" si="4"/>
+        <v>0.52200000000000002</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A296">
         <v>46.612000000000002</v>
       </c>
       <c r="B296">
         <v>26.8</v>
       </c>
-    </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C296">
+        <f t="shared" si="4"/>
+        <v>0.53600000000000003</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A297">
         <v>46.816000000000003</v>
       </c>
       <c r="B297">
         <v>25.4</v>
       </c>
-    </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C297">
+        <f t="shared" si="4"/>
+        <v>0.50800000000000001</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A298">
         <v>46.915999999999997</v>
       </c>
       <c r="B298">
         <v>26.1</v>
       </c>
-    </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C298">
+        <f t="shared" si="4"/>
+        <v>0.52200000000000002</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A299">
         <v>47.118000000000002</v>
       </c>
       <c r="B299">
         <v>24.6</v>
       </c>
-    </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C299">
+        <f t="shared" si="4"/>
+        <v>0.49200000000000005</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A300">
         <v>47.427</v>
       </c>
       <c r="B300">
         <v>25.7</v>
       </c>
-    </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C300">
+        <f t="shared" si="4"/>
+        <v>0.51400000000000001</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A301">
         <v>47.832000000000001</v>
       </c>
       <c r="B301">
         <v>23.3</v>
       </c>
-    </row>
-    <row r="302" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C301">
+        <f t="shared" si="4"/>
+        <v>0.46600000000000003</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A302">
         <v>48.034999999999997</v>
       </c>
       <c r="B302">
         <v>23.7</v>
       </c>
-    </row>
-    <row r="303" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C302">
+        <f t="shared" si="4"/>
+        <v>0.47399999999999998</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A303">
         <v>48.134999999999998</v>
       </c>
       <c r="B303">
         <v>24.6</v>
       </c>
-    </row>
-    <row r="304" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C303">
+        <f t="shared" si="4"/>
+        <v>0.49200000000000005</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A304">
         <v>48.237000000000002</v>
       </c>
       <c r="B304">
         <v>25.6</v>
       </c>
-    </row>
-    <row r="305" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C304">
+        <f t="shared" si="4"/>
+        <v>0.51200000000000001</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A305">
         <v>48.335999999999999</v>
       </c>
       <c r="B305">
         <v>25.8</v>
       </c>
-    </row>
-    <row r="306" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C305">
+        <f t="shared" si="4"/>
+        <v>0.51600000000000001</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A306">
         <v>48.436999999999998</v>
       </c>
       <c r="B306">
         <v>25.4</v>
       </c>
-    </row>
-    <row r="307" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C306">
+        <f t="shared" si="4"/>
+        <v>0.50800000000000001</v>
+      </c>
+    </row>
+    <row r="307" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A307">
         <v>48.536999999999999</v>
       </c>
       <c r="B307">
         <v>24.9</v>
       </c>
-    </row>
-    <row r="308" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C307">
+        <f t="shared" si="4"/>
+        <v>0.498</v>
+      </c>
+    </row>
+    <row r="308" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A308">
         <v>48.637</v>
       </c>
       <c r="B308">
         <v>25.9</v>
       </c>
-    </row>
-    <row r="309" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C308">
+        <f t="shared" si="4"/>
+        <v>0.51800000000000002</v>
+      </c>
+    </row>
+    <row r="309" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A309">
         <v>48.735999999999997</v>
       </c>
       <c r="B309">
         <v>25.6</v>
       </c>
-    </row>
-    <row r="310" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C309">
+        <f t="shared" si="4"/>
+        <v>0.51200000000000001</v>
+      </c>
+    </row>
+    <row r="310" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A310">
         <v>48.835000000000001</v>
       </c>
       <c r="B310">
         <v>25.7</v>
       </c>
-    </row>
-    <row r="311" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C310">
+        <f t="shared" si="4"/>
+        <v>0.51400000000000001</v>
+      </c>
+    </row>
+    <row r="311" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A311">
         <v>48.933999999999997</v>
       </c>
       <c r="B311">
         <v>26.2</v>
+      </c>
+      <c r="C311">
+        <f t="shared" si="4"/>
+        <v>0.52400000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>